<commit_message>
CRUD operation of Learning Journey on 29MAY2025
</commit_message>
<xml_diff>
--- a/Utility/LPEXCEL.xlsx
+++ b/Utility/LPEXCEL.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sevvelkaranpalanivetrivel/Desktop/PILOT/Smartcliff_RobotFramework_Project/Utility/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sevvelkaranpalanivetrivel/Desktop/PILOT/Smartcliff_RobotFramework_Project-1/Utility/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8335F4FD-44F7-214E-9F97-1EC92062E26F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C7EF1D-6A8E-F64C-B767-FF1C706038B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16220" xr2:uid="{AF9B29BB-B471-8D40-B4EF-89889A3C9874}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
   <si>
     <t>${title}</t>
   </si>
@@ -422,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7072C98E-9D33-A24F-A7F2-31D1C9920839}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -496,6 +496,20 @@
         <v>7</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>